<commit_message>
[Inheritance and Interfaces] Extending class
</commit_message>
<xml_diff>
--- a/ChartBuilder/Files/Bench Press M0.xlsx
+++ b/ChartBuilder/Files/Bench Press M0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akhilesh Pc\Documents\Git\Kotlin\ChartBuilder\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8190551E-00F9-42A2-9E01-F4704D83733C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592D17BB-A53F-4B96-958F-DA9FD92B39DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16566" windowHeight="5253" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>WEEK 1</t>
   </si>
@@ -83,6 +83,30 @@
   </si>
   <si>
     <t>20x2, 2.5x1</t>
+  </si>
+  <si>
+    <t>20x1, 10x1, 5x1</t>
+  </si>
+  <si>
+    <t>20x2</t>
+  </si>
+  <si>
+    <t>20x2, 5x1</t>
+  </si>
+  <si>
+    <t>20x2, 1x2.5</t>
+  </si>
+  <si>
+    <t>20x2, 5x1, 2.5x1</t>
+  </si>
+  <si>
+    <t>1x20</t>
+  </si>
+  <si>
+    <t>1x20, 1x5</t>
+  </si>
+  <si>
+    <t>1x20, 1x10</t>
   </si>
 </sst>
 </file>
@@ -437,7 +461,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,6 +520,9 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
@@ -504,6 +531,9 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
@@ -512,6 +542,9 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -525,6 +558,9 @@
       <c r="C14" t="s">
         <v>4</v>
       </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
@@ -533,6 +569,9 @@
       <c r="C15" t="s">
         <v>12</v>
       </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -541,34 +580,46 @@
       <c r="C16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>1</v>
       </c>
       <c r="C20" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>3</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>5</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>